<commit_message>
Added Fusion Archive Files
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca Desktop\Documents\GitHub\MilwaukeeM18-2-CarJack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca Thinkpad\Documents\GitHub\MilwaukeeM18-2-CarJack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A8F474-63DE-4CD2-BEC4-D5B81B988A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC05F71B-5BBF-4B28-9AE1-9349AB134721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="600" windowWidth="25800" windowHeight="21000" xr2:uid="{B81C6F19-3F67-4DC4-A35B-199AB7048977}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{B81C6F19-3F67-4DC4-A35B-199AB7048977}"/>
   </bookViews>
   <sheets>
     <sheet name="Komparator mit Hysterese" sheetId="1" r:id="rId1"/>
+    <sheet name="SIC431" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>low</t>
   </si>
@@ -78,6 +79,72 @@
   </si>
   <si>
     <t>V_THR-off</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>f_sw</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>L-Ripple</t>
+  </si>
+  <si>
+    <t>kOhm</t>
+  </si>
+  <si>
+    <t>R_FB_L</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>C_in_min</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>V_pk</t>
+  </si>
+  <si>
+    <t>C_out_min</t>
+  </si>
+  <si>
+    <t>V_FB</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>L_out</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>I_out_rip</t>
+  </si>
+  <si>
+    <t>I_out_max</t>
+  </si>
+  <si>
+    <t>DutyCycle</t>
+  </si>
+  <si>
+    <t>V_out</t>
+  </si>
+  <si>
+    <t>R_FB_H</t>
+  </si>
+  <si>
+    <t>V_in</t>
   </si>
 </sst>
 </file>
@@ -103,12 +170,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -124,15 +203,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -197,7 +279,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -495,13 +577,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34210484-A071-4D78-B42F-FECE05B7234E}">
   <dimension ref="A2:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -521,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -535,7 +617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -551,11 +633,11 @@
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2">
-        <f t="shared" ref="H4:I4" si="0">D3/$C$6</f>
+        <f t="shared" ref="I4" si="0">D3/$C$6</f>
         <v>180000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -575,7 +657,7 @@
         <v>81999.999999999985</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -592,11 +674,11 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1">
-        <f t="shared" ref="H6:I6" si="1">((D$3-$C$5)*I$4)/D$3</f>
+        <f t="shared" ref="I6" si="1">((D$3-$C$5)*I$4)/D$3</f>
         <v>98000.000000000015</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -606,15 +688,15 @@
       <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <f>$C$5*(1+($G6/((G5*C7)/(G5+C7))))</f>
         <v>18.262600000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G9" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -627,4 +709,177 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BD2FCF-1518-4831-9D6B-47BCE21FE848}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="5">
+        <f>($C$12*($C$3-$C$7))/$C$7</f>
+        <v>104.96666666666668</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="5">
+        <f>$C$3/$C$2</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5">
+        <f>C4*C13/100</f>
+        <v>7.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="5">
+        <f>((C2-C3)*G3)/(C13*C4*C15)</f>
+        <v>1.2444444444444443E-5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>0.6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5">
+        <f>((G5*(C4+0.5*C5)^2))/(C8^2-C3^2)</f>
+        <v>1.7857142857142855E-5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C2</f>
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1">
+        <f>C4*(G3*(1-G3))/(C2*C15)</f>
+        <v>3.1746031746031746E-4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3">
+        <v>500</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New optional mosfets, Thermal Vias under SIC431, minor layout changes
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca Thinkpad\Documents\GitHub\MilwaukeeM18-2-CarJack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca Desktop\Documents\GitHub\MilwaukeeM18-2-CarJack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC05F71B-5BBF-4B28-9AE1-9349AB134721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93A9113-EDE8-47D3-8CF3-9BFE3CC892CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{B81C6F19-3F67-4DC4-A35B-199AB7048977}"/>
+    <workbookView xWindow="3510" yWindow="4110" windowWidth="14970" windowHeight="14805" activeTab="1" xr2:uid="{B81C6F19-3F67-4DC4-A35B-199AB7048977}"/>
   </bookViews>
   <sheets>
     <sheet name="Komparator mit Hysterese" sheetId="1" r:id="rId1"/>
@@ -213,8 +213,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -581,9 +581,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -617,7 +617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -637,7 +637,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -657,7 +657,7 @@
         <v>81999.999999999985</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -678,7 +678,7 @@
         <v>98000.000000000015</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -693,10 +693,10 @@
         <v>18.262600000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -716,17 +716,17 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -747,7 +747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -768,7 +768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -779,7 +779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>30</v>
       </c>
@@ -801,7 +801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -822,7 +822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -834,7 +834,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>22</v>
       </c>
@@ -846,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -857,7 +857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -868,7 +868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>

</xml_diff>